<commit_message>
Completed Post Batch request
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anbum\OneDrive\Desktop\Anbu\LMS_Phase2_RestAssured\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anbum\OneDrive\Desktop\Anbu\LMS_Phase2_RestAssured\LMS_GIT\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16F7D609-006B-4D8E-A60C-D190B8321281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121FE320-246B-4D64-B0C5-48D24732B15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch" sheetId="1" r:id="rId1"/>
-    <sheet name="Program" sheetId="2" r:id="rId2"/>
-    <sheet name="Class" sheetId="3" r:id="rId3"/>
+    <sheet name="GetAllBatches" sheetId="4" r:id="rId2"/>
+    <sheet name="Program" sheetId="2" r:id="rId3"/>
+    <sheet name="Class" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
   <si>
     <t>TestCase</t>
   </si>
@@ -89,9 +90,6 @@
     <t>Missing mandatory fields</t>
   </si>
   <si>
-    <t>Missing additional fields</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Invalid data in request body</t>
   </si>
   <si>
@@ -101,12 +99,6 @@
     <t>Invalid BaseURL</t>
   </si>
   <si>
-    <t>Invalid Method</t>
-  </si>
-  <si>
-    <t>Only with Madatory fields</t>
-  </si>
-  <si>
     <t>Test1</t>
   </si>
   <si>
@@ -165,13 +157,125 @@
   </si>
   <si>
     <t>ExpStatusCode</t>
+  </si>
+  <si>
+    <r>
+      <t>GETALL_BATCH_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GETALL_BATCH_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <r>
+      <t>GETALL_BATCH_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>02</t>
+    </r>
+  </si>
+  <si>
+    <t>First Test</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Test13426</t>
+  </si>
+  <si>
+    <t>Test78Testin</t>
+  </si>
+  <si>
+    <t>POST-BATCH-08</t>
+  </si>
+  <si>
+    <t>Valid Data</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Testing  Description</t>
+  </si>
+  <si>
+    <t>2334</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Only mandatory fields</t>
+  </si>
+  <si>
+    <t>17470</t>
+  </si>
+  <si>
+    <t>Mandatory Field</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>bat$$$</t>
+  </si>
+  <si>
+    <t>TestingCreate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +294,24 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,12 +334,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,20 +622,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
@@ -539,7 +663,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -551,10 +675,10 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -562,28 +686,31 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="M2" t="s">
         <v>16</v>
@@ -594,28 +721,31 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="M3" t="s">
         <v>17</v>
@@ -626,28 +756,31 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
@@ -658,16 +791,19 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="M5" t="s">
         <v>19</v>
@@ -678,13 +814,29 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -692,13 +844,34 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="M7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -706,28 +879,94 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="M8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M10" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M12" t="s">
-        <v>25</v>
+      <c r="A11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -738,6 +977,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6315C3-6D77-4A11-80D2-ECD0EA9C6857}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -749,7 +1045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Data Driven changes for Program module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\eclipse-workspace\Team4_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABBBE65-A0CF-4B35-BA1F-80A9B9136D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304C5737-2E05-411F-AE06-217B013C53A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,185 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>BaseURL</t>
+  </si>
+  <si>
+    <t>batchName</t>
+  </si>
+  <si>
+    <t>batchDescription</t>
+  </si>
+  <si>
+    <t>batchStatus</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>POST-BATCH-01</t>
+  </si>
+  <si>
+    <t>POST-BATCH-02</t>
+  </si>
+  <si>
+    <t>POST-BATCH-03</t>
+  </si>
+  <si>
+    <t>POST-BATCH-04</t>
+  </si>
+  <si>
+    <t>POST-BATCH-05</t>
+  </si>
+  <si>
+    <t>POST-BATCH-06</t>
+  </si>
+  <si>
+    <t>POST-BATCH-07</t>
+  </si>
+  <si>
+    <t>Invalid Endpoint</t>
+  </si>
+  <si>
+    <t>Without Authorization</t>
+  </si>
+  <si>
+    <t>Existing batch details</t>
+  </si>
+  <si>
+    <t>Missing mandatory fields</t>
+  </si>
+  <si>
+    <t>Missing additional fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Invalid data in request body</t>
+  </si>
+  <si>
+    <t>Inactive program ID</t>
+  </si>
+  <si>
+    <t>Invalid BaseURL</t>
+  </si>
+  <si>
+    <t>Invalid Method</t>
+  </si>
+  <si>
+    <t>Only with Madatory fields</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>NoOfClasses</t>
+  </si>
+  <si>
+    <t>Anbu</t>
+  </si>
+  <si>
+    <t>Aru</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>1245</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>TestingBUG</t>
+  </si>
+  <si>
+    <t>16262</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10</t>
+  </si>
+  <si>
+    <t>Authorizarion</t>
+  </si>
+  <si>
+    <t>InvalidEndpoint</t>
+  </si>
+  <si>
+    <t>InValid</t>
+  </si>
+  <si>
+    <t>RestAssured Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Missing Mandatory fields</t>
+  </si>
+  <si>
+    <t>ExpStatusCode</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Avengers</t>
+  </si>
+  <si>
+    <t>TestC</t>
+  </si>
+  <si>
+    <t>JavaX</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -36,16 +212,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -53,12 +260,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,6 +600,342 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" customWidth="1"/>
+    <col min="11" max="12" width="15.88671875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1234</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -347,28 +944,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Endpoint column in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304C5737-2E05-411F-AE06-217B013C53A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAE8061-0F8D-4B00-859F-C300555B6382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
   <si>
     <t>TestCase</t>
   </si>
@@ -185,26 +185,101 @@
     <t>TC02</t>
   </si>
   <si>
-    <t>Invalid</t>
-  </si>
-  <si>
     <t>400</t>
   </si>
   <si>
-    <t>Avengers</t>
-  </si>
-  <si>
-    <t>TestC</t>
-  </si>
-  <si>
     <t>JavaX</t>
+  </si>
+  <si>
+    <t>/saveprogram</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>Valid With Mandatory Details</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>AvgQA</t>
+  </si>
+  <si>
+    <t>TestQ</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>/save</t>
+  </si>
+  <si>
+    <t>Invalid endpoint</t>
+  </si>
+  <si>
+    <t>Invalid Program Desc</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>AvgQAA</t>
+  </si>
+  <si>
+    <t>AvgQAB</t>
+  </si>
+  <si>
+    <t>Invalid -Already Existing Program Name</t>
+  </si>
+  <si>
+    <t>Invalid Method -Mentioned in feature file</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>Invalid Request Body</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>123@#$</t>
+  </si>
+  <si>
+    <t>Invalid Program Name</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Invalid Program Status</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>Invalid -No Auth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +312,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -252,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -282,46 +365,65 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -841,10 +943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,82 +956,261 @@
     <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="G2" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D3" s="6">
+        <v>1234</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="B4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="F4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="8" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="8">
-        <v>1234</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="C11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>36</v>
+      <c r="F11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{1ABA59E8-9459-41C9-BF54-78391EB45490}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Data Driven For Class Module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\eclipse-workspace\Team4_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LaksA\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABBBE65-A0CF-4B35-BA1F-80A9B9136D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B1AA5F-395B-42C4-B7CE-4DC5602039CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>U49</t>
+  </si>
+  <si>
+    <t>TestAlluree</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Classno</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Classdate</t>
+  </si>
+  <si>
+    <t>Batchname</t>
+  </si>
+  <si>
+    <t>Staffname</t>
+  </si>
+  <si>
+    <t>Classtopic</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57,8 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,7 +376,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -355,7 +388,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -363,12 +396,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8547</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45649</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Get all programs features and steps testData case updated in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\eclipse-workspace\Team4_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABBBE65-A0CF-4B35-BA1F-80A9B9136D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5310D4E3-D8F1-4110-ADB5-84633B22DC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Batch" sheetId="1" r:id="rId1"/>
-    <sheet name="Program" sheetId="2" r:id="rId2"/>
-    <sheet name="Class" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="4" r:id="rId1"/>
+    <sheet name="Batch" sheetId="1" r:id="rId2"/>
+    <sheet name="Program" sheetId="2" r:id="rId3"/>
+    <sheet name="Class" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,9 +27,242 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>BaseURL</t>
+  </si>
+  <si>
+    <t>batchName</t>
+  </si>
+  <si>
+    <t>batchDescription</t>
+  </si>
+  <si>
+    <t>batchStatus</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>POST-BATCH-01</t>
+  </si>
+  <si>
+    <t>POST-BATCH-02</t>
+  </si>
+  <si>
+    <t>POST-BATCH-03</t>
+  </si>
+  <si>
+    <t>POST-BATCH-04</t>
+  </si>
+  <si>
+    <t>POST-BATCH-05</t>
+  </si>
+  <si>
+    <t>POST-BATCH-06</t>
+  </si>
+  <si>
+    <t>POST-BATCH-07</t>
+  </si>
+  <si>
+    <t>Invalid Endpoint</t>
+  </si>
+  <si>
+    <t>Without Authorization</t>
+  </si>
+  <si>
+    <t>Existing batch details</t>
+  </si>
+  <si>
+    <t>Missing mandatory fields</t>
+  </si>
+  <si>
+    <t>Missing additional fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Invalid data in request body</t>
+  </si>
+  <si>
+    <t>Inactive program ID</t>
+  </si>
+  <si>
+    <t>Invalid BaseURL</t>
+  </si>
+  <si>
+    <t>Invalid Method</t>
+  </si>
+  <si>
+    <t>Only with Madatory fields</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>NoOfClasses</t>
+  </si>
+  <si>
+    <t>Anbu</t>
+  </si>
+  <si>
+    <t>Aru</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>1245</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>TestingBUG</t>
+  </si>
+  <si>
+    <t>16262</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10</t>
+  </si>
+  <si>
+    <t>Authorizarion</t>
+  </si>
+  <si>
+    <t>InvalidEndpoint</t>
+  </si>
+  <si>
+    <t>InValid</t>
+  </si>
+  <si>
+    <t>RestAssured Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Missing Mandatory fields</t>
+  </si>
+  <si>
+    <t>ExpStatusCode</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Avengers</t>
+  </si>
+  <si>
+    <t>TestC</t>
+  </si>
+  <si>
+    <t>JavaX</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Base URL</t>
+  </si>
+  <si>
+    <t>End Point</t>
+  </si>
+  <si>
+    <t>Mehtod</t>
+  </si>
+  <si>
+    <t>Expected Code</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>TC-01</t>
+  </si>
+  <si>
+    <t>TC-02</t>
+  </si>
+  <si>
+    <t>https://lms-hackthon-oct24-3efc7e0df381.herokuapp.com/lms</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>sdet@gmail.com</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi@2024</t>
+  </si>
+  <si>
+    <t>Assertion</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi@2025</t>
+  </si>
+  <si>
+    <t>TC-03</t>
+  </si>
+  <si>
+    <t>/loginInvalid</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -36,16 +270,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -53,14 +332,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -338,36 +678,484 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38B70D3-B77B-4775-B7D9-2B54CF1A978A}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3">
+        <v>401</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4">
+        <v>400</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="12" width="15.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1234</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated testData.xlsx with Manali's chagnes and my changes.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64E6C2A-D788-476B-A95C-102B4861708F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADFCA5B-0E32-44D7-92E3-638149E636C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Batch" sheetId="1" r:id="rId1"/>
-    <sheet name="Program" sheetId="2" r:id="rId2"/>
-    <sheet name="Class" sheetId="3" r:id="rId3"/>
+    <sheet name="LogIn-LogOut" sheetId="4" r:id="rId1"/>
+    <sheet name="Batch" sheetId="1" r:id="rId2"/>
+    <sheet name="Program" sheetId="2" r:id="rId3"/>
+    <sheet name="Class" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="136">
   <si>
     <t>TestCase</t>
   </si>
@@ -378,13 +379,70 @@
   </si>
   <si>
     <t>Program2</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Base URL</t>
+  </si>
+  <si>
+    <t>End Point</t>
+  </si>
+  <si>
+    <t>Mehtod</t>
+  </si>
+  <si>
+    <t>Expected Code</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Assertion</t>
+  </si>
+  <si>
+    <t>TC-01</t>
+  </si>
+  <si>
+    <t>https://lms-hackthon-oct24-3efc7e0df381.herokuapp.com/lms</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>sdet@gmail.com</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi@2024</t>
+  </si>
+  <si>
+    <t>TC-02</t>
+  </si>
+  <si>
+    <t>/loginInvalid</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi@2025</t>
+  </si>
+  <si>
+    <t>TC-03</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +482,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -522,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -546,6 +610,9 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -826,6 +893,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7F8A30-0F06-4386-B231-CDAB3429D422}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3">
+        <v>401</v>
+      </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4">
+        <v>400</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
@@ -833,22 +1029,22 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" customWidth="1"/>
-    <col min="11" max="12" width="15.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="12" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -886,7 +1082,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -918,7 +1114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -950,7 +1146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -982,7 +1178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1002,7 +1198,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1016,7 +1212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1030,7 +1226,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1044,17 +1240,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
         <v>25</v>
       </c>
@@ -1066,26 +1262,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -1108,7 +1304,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>83</v>
       </c>
@@ -1134,7 +1330,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
@@ -1157,7 +1353,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>85</v>
       </c>
@@ -1181,7 +1377,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>86</v>
       </c>
@@ -1204,7 +1400,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>87</v>
       </c>
@@ -1227,7 +1423,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>88</v>
       </c>
@@ -1250,7 +1446,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>89</v>
       </c>
@@ -1273,7 +1469,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>90</v>
       </c>
@@ -1292,7 +1488,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>91</v>
       </c>
@@ -1315,7 +1511,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>92</v>
       </c>
@@ -1338,7 +1534,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>93</v>
       </c>
@@ -1355,7 +1551,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>94</v>
       </c>
@@ -1372,7 +1568,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>95</v>
       </c>
@@ -1389,7 +1585,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>96</v>
       </c>
@@ -1406,7 +1602,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>97</v>
       </c>
@@ -1423,7 +1619,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>98</v>
       </c>
@@ -1440,7 +1636,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>99</v>
       </c>
@@ -1457,7 +1653,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>100</v>
       </c>
@@ -1474,7 +1670,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>101</v>
       </c>
@@ -1491,7 +1687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>102</v>
       </c>
@@ -1508,7 +1704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>103</v>
       </c>
@@ -1525,7 +1721,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>104</v>
       </c>
@@ -1542,7 +1738,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>105</v>
       </c>
@@ -1559,7 +1755,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>107</v>
       </c>
@@ -1579,7 +1775,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>108</v>
       </c>
@@ -1599,7 +1795,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>109</v>
       </c>
@@ -1617,7 +1813,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>110</v>
       </c>
@@ -1637,7 +1833,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>111</v>
       </c>
@@ -1657,7 +1853,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>112</v>
       </c>
@@ -1677,7 +1873,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>113</v>
       </c>
@@ -1705,13 +1901,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added scenarios for PUT program
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64E6C2A-D788-476B-A95C-102B4861708F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A72B2DC-C4E9-4636-844C-4F5350AA7388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="122">
   <si>
     <t>TestCase</t>
   </si>
@@ -378,6 +378,21 @@
   </si>
   <si>
     <t>Program2</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>RubyAPI</t>
+  </si>
+  <si>
+    <t>TestS</t>
+  </si>
+  <si>
+    <t>Wells</t>
+  </si>
+  <si>
+    <t>Fargo</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1086,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,13 +1128,13 @@
         <v>83</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>46</v>
@@ -1139,22 +1154,23 @@
         <v>84</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="11">
-        <v>1234</v>
-      </c>
+      <c r="D3" s="11"/>
       <c r="E3" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1162,23 +1178,22 @@
         <v>85</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="11"/>
+      <c r="D4" s="11">
+        <v>1234</v>
+      </c>
       <c r="E4" s="11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" t="s">
-        <v>116</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1564,16 +1579,16 @@
         <v>107</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>55</v>
+        <v>118</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Completed changes using excel, Data Driven: Login scenarios Logout scenarios Get All Program/ID/User scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADFCA5B-0E32-44D7-92E3-638149E636C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C7A22F-9AD1-4618-BF77-3611391DC6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn-LogOut" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="151">
   <si>
     <t>TestCase</t>
   </si>
@@ -390,9 +390,6 @@
     <t>End Point</t>
   </si>
   <si>
-    <t>Mehtod</t>
-  </si>
-  <si>
     <t>Expected Code</t>
   </si>
   <si>
@@ -402,40 +399,88 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Assertion</t>
-  </si>
-  <si>
-    <t>TC-01</t>
-  </si>
-  <si>
     <t>https://lms-hackthon-oct24-3efc7e0df381.herokuapp.com/lms</t>
   </si>
   <si>
     <t>/login</t>
   </si>
   <si>
-    <t>POST</t>
-  </si>
-  <si>
     <t>sdet@gmail.com</t>
   </si>
   <si>
     <t>LmsHackathonApi@2024</t>
   </si>
   <si>
-    <t>TC-02</t>
-  </si>
-  <si>
     <t>/loginInvalid</t>
   </si>
   <si>
     <t>LmsHackathonApi@2025</t>
   </si>
   <si>
-    <t>TC-03</t>
-  </si>
-  <si>
     <t>LmsHackathonApi</t>
+  </si>
+  <si>
+    <t>POST_LOGIN-01</t>
+  </si>
+  <si>
+    <t>POST_LOGIN-02</t>
+  </si>
+  <si>
+    <t>POST_LOGIN-03</t>
+  </si>
+  <si>
+    <t>/logoutlms</t>
+  </si>
+  <si>
+    <t>/logoutlmsInvalid</t>
+  </si>
+  <si>
+    <t>Invalid - No Auth</t>
+  </si>
+  <si>
+    <t>Invalid - Invalid endpoint</t>
+  </si>
+  <si>
+    <t>InValid - Invalid credentials</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>GET_LOGOUT-04</t>
+  </si>
+  <si>
+    <t>GET_LOGOUT-05</t>
+  </si>
+  <si>
+    <t>GET_LOGOUT-06</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>StoreToken</t>
+  </si>
+  <si>
+    <t>NoAuth</t>
+  </si>
+  <si>
+    <t>WithAuth</t>
+  </si>
+  <si>
+    <t>AddProgramId</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>/allProgramsWithUsers1</t>
+  </si>
+  <si>
+    <t>AddProgramId,NoAuth</t>
+  </si>
+  <si>
+    <t>AddProgramId,InvalidUri</t>
   </si>
 </sst>
 </file>
@@ -586,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -611,6 +656,10 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -894,22 +943,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7F8A30-0F06-4386-B231-CDAB3429D422}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -932,33 +981,33 @@
         <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="H1" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="F2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2">
-        <v>200</v>
-      </c>
-      <c r="F2" t="s">
-        <v>129</v>
-      </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="H2" t="s">
         <v>36</v>
@@ -968,55 +1017,110 @@
       <c r="A3" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>126</v>
+      <c r="B3" s="19" t="s">
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3">
+        <v>401</v>
+      </c>
+      <c r="E3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" t="s">
         <v>128</v>
       </c>
-      <c r="E3">
-        <v>401</v>
-      </c>
-      <c r="F3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" t="s">
-        <v>133</v>
-      </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4">
+        <v>124</v>
+      </c>
+      <c r="D4">
         <v>400</v>
+      </c>
+      <c r="E4" t="s">
+        <v>125</v>
       </c>
       <c r="F4" t="s">
         <v>129</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="G5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6">
+        <v>404</v>
+      </c>
+      <c r="G6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7">
+        <v>401</v>
+      </c>
+      <c r="H7" t="s">
         <v>135</v>
       </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{8542BF74-EF46-40D0-B744-00A12192AD89}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1264,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,10 +1382,11 @@
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -1301,10 +1406,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>83</v>
       </c>
@@ -1323,14 +1434,16 @@
       <c r="F2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="J2" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
@@ -1349,11 +1462,13 @@
       <c r="F3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>85</v>
       </c>
@@ -1370,14 +1485,16 @@
       <c r="F4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>86</v>
       </c>
@@ -1396,11 +1513,13 @@
       <c r="F5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>87</v>
       </c>
@@ -1419,11 +1538,13 @@
       <c r="F6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>88</v>
       </c>
@@ -1442,11 +1563,13 @@
       <c r="F7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>89</v>
       </c>
@@ -1465,11 +1588,13 @@
       <c r="F8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>90</v>
       </c>
@@ -1484,11 +1609,13 @@
       <c r="F9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>91</v>
       </c>
@@ -1507,11 +1634,13 @@
       <c r="F10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>92</v>
       </c>
@@ -1530,11 +1659,13 @@
       <c r="F11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>93</v>
       </c>
@@ -1547,11 +1678,13 @@
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>94</v>
       </c>
@@ -1564,11 +1697,13 @@
       <c r="F13" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>95</v>
       </c>
@@ -1581,11 +1716,15 @@
       <c r="F14" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>96</v>
       </c>
@@ -1598,11 +1737,15 @@
       <c r="F15" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>97</v>
       </c>
@@ -1616,10 +1759,14 @@
         <v>77</v>
       </c>
       <c r="G16" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>98</v>
       </c>
@@ -1632,11 +1779,13 @@
       <c r="F17" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>99</v>
       </c>
@@ -1649,11 +1798,15 @@
       <c r="F18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>100</v>
       </c>
@@ -1667,10 +1820,14 @@
         <v>77</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>101</v>
       </c>
@@ -1683,11 +1840,13 @@
       <c r="F20" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="8"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>102</v>
       </c>
@@ -1700,11 +1859,13 @@
       <c r="F21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="8"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>103</v>
       </c>
@@ -1715,13 +1876,15 @@
         <v>58</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>104</v>
       </c>
@@ -1734,11 +1897,15 @@
       <c r="F23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="8"/>
+      <c r="H23" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>105</v>
       </c>
@@ -1752,10 +1919,14 @@
         <v>82</v>
       </c>
       <c r="G24" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>107</v>
       </c>
@@ -1774,8 +1945,10 @@
       <c r="F25" s="11" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>108</v>
       </c>
@@ -1794,8 +1967,10 @@
       <c r="F26" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>109</v>
       </c>
@@ -1812,8 +1987,10 @@
       <c r="F27" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>110</v>
       </c>
@@ -1832,8 +2009,10 @@
       <c r="F28" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>111</v>
       </c>
@@ -1852,8 +2031,10 @@
       <c r="F29" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>112</v>
       </c>
@@ -1872,8 +2053,10 @@
       <c r="F30" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>113</v>
       </c>
@@ -1892,12 +2075,15 @@
       <c r="F31" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{1ABA59E8-9459-41C9-BF54-78391EB45490}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Resolved merge issues Merged excel with Manali's branch
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A72B2DC-C4E9-4636-844C-4F5350AA7388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4BB9CD-9799-474E-8926-C7AD20BD4B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Batch" sheetId="1" r:id="rId1"/>
-    <sheet name="Program" sheetId="2" r:id="rId2"/>
-    <sheet name="Class" sheetId="3" r:id="rId3"/>
+    <sheet name="LogIn-LogOut" sheetId="4" r:id="rId1"/>
+    <sheet name="Batch" sheetId="1" r:id="rId2"/>
+    <sheet name="Program" sheetId="2" r:id="rId3"/>
+    <sheet name="Class" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="155">
   <si>
     <t>TestCase</t>
   </si>
@@ -393,13 +394,112 @@
   </si>
   <si>
     <t>Fargo</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>NoAuth</t>
+  </si>
+  <si>
+    <t>AddProgramId</t>
+  </si>
+  <si>
+    <t>AddProgramId,InvalidUri</t>
+  </si>
+  <si>
+    <t>AddProgramId,NoAuth</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Base URL</t>
+  </si>
+  <si>
+    <t>End Point</t>
+  </si>
+  <si>
+    <t>Expected Code</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>POST_LOGIN-01</t>
+  </si>
+  <si>
+    <t>https://lms-hackthon-oct24-3efc7e0df381.herokuapp.com/lms</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>sdet@gmail.com</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi@2024</t>
+  </si>
+  <si>
+    <t>StoreToken</t>
+  </si>
+  <si>
+    <t>POST_LOGIN-02</t>
+  </si>
+  <si>
+    <t>/loginInvalid</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi@2025</t>
+  </si>
+  <si>
+    <t>Invalid - Invalid endpoint</t>
+  </si>
+  <si>
+    <t>POST_LOGIN-03</t>
+  </si>
+  <si>
+    <t>LmsHackathonApi</t>
+  </si>
+  <si>
+    <t>InValid - Invalid credentials</t>
+  </si>
+  <si>
+    <t>GET_LOGOUT-04</t>
+  </si>
+  <si>
+    <t>/logoutlms</t>
+  </si>
+  <si>
+    <t>WithAuth</t>
+  </si>
+  <si>
+    <t>GET_LOGOUT-05</t>
+  </si>
+  <si>
+    <t>/logoutlmsInvalid</t>
+  </si>
+  <si>
+    <t>GET_LOGOUT-06</t>
+  </si>
+  <si>
+    <t>Invalid - No Auth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,6 +539,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -537,7 +643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -561,6 +667,13 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -841,6 +954,189 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D65F20-97A6-4250-B793-700476770169}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3">
+        <v>401</v>
+      </c>
+      <c r="E3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="G5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6">
+        <v>404</v>
+      </c>
+      <c r="G6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7">
+        <v>401</v>
+      </c>
+      <c r="H7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{EC63BFB6-1B64-4208-8A24-E7F266E28780}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
@@ -848,22 +1144,22 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" customWidth="1"/>
-    <col min="11" max="12" width="15.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="12" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -901,7 +1197,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -933,7 +1229,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -965,7 +1261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -997,7 +1293,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1017,7 +1313,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1031,7 +1327,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1045,7 +1341,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1059,17 +1355,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
         <v>25</v>
       </c>
@@ -1081,26 +1377,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -1120,10 +1417,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>83</v>
       </c>
@@ -1142,14 +1445,16 @@
       <c r="F2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="J2" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
@@ -1166,14 +1471,16 @@
       <c r="F3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>85</v>
       </c>
@@ -1192,11 +1499,13 @@
       <c r="F4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>86</v>
       </c>
@@ -1215,11 +1524,13 @@
       <c r="F5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>87</v>
       </c>
@@ -1238,11 +1549,13 @@
       <c r="F6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>88</v>
       </c>
@@ -1261,11 +1574,13 @@
       <c r="F7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>89</v>
       </c>
@@ -1284,11 +1599,13 @@
       <c r="F8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>90</v>
       </c>
@@ -1303,11 +1620,13 @@
       <c r="F9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>91</v>
       </c>
@@ -1326,11 +1645,13 @@
       <c r="F10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>92</v>
       </c>
@@ -1349,11 +1670,13 @@
       <c r="F11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>93</v>
       </c>
@@ -1366,11 +1689,13 @@
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>94</v>
       </c>
@@ -1383,11 +1708,13 @@
       <c r="F13" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>95</v>
       </c>
@@ -1400,11 +1727,15 @@
       <c r="F14" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>96</v>
       </c>
@@ -1417,11 +1748,15 @@
       <c r="F15" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>97</v>
       </c>
@@ -1435,10 +1770,14 @@
         <v>77</v>
       </c>
       <c r="G16" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>98</v>
       </c>
@@ -1451,11 +1790,13 @@
       <c r="F17" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>99</v>
       </c>
@@ -1468,11 +1809,15 @@
       <c r="F18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>100</v>
       </c>
@@ -1486,10 +1831,14 @@
         <v>77</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>101</v>
       </c>
@@ -1502,11 +1851,13 @@
       <c r="F20" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="8"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>102</v>
       </c>
@@ -1519,11 +1870,13 @@
       <c r="F21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="8"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>103</v>
       </c>
@@ -1536,11 +1889,13 @@
       <c r="F22" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="8"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>104</v>
       </c>
@@ -1553,11 +1908,15 @@
       <c r="F23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="8"/>
+      <c r="H23" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>105</v>
       </c>
@@ -1571,10 +1930,14 @@
         <v>82</v>
       </c>
       <c r="G24" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>107</v>
       </c>
@@ -1593,8 +1956,10 @@
       <c r="F25" s="11" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>108</v>
       </c>
@@ -1613,8 +1978,10 @@
       <c r="F26" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>109</v>
       </c>
@@ -1631,8 +1998,10 @@
       <c r="F27" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>110</v>
       </c>
@@ -1651,8 +2020,10 @@
       <c r="F28" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>111</v>
       </c>
@@ -1671,8 +2042,10 @@
       <c r="F29" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>112</v>
       </c>
@@ -1691,8 +2064,10 @@
       <c r="F30" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>113</v>
       </c>
@@ -1711,6 +2086,8 @@
       <c r="F31" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1720,13 +2097,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fINAL COMMIT FOR LOGIN,LOGINOUT,GET ALL PROGRAM/ID/USER
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4BB9CD-9799-474E-8926-C7AD20BD4B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FCEA05-45CF-4BED-A357-63FE0A386906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn-LogOut" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="155">
   <si>
     <t>TestCase</t>
   </si>
@@ -381,18 +381,12 @@
     <t>Program2</t>
   </si>
   <si>
-    <t>tester</t>
-  </si>
-  <si>
     <t>RubyAPI</t>
   </si>
   <si>
     <t>TestS</t>
   </si>
   <si>
-    <t>Wells</t>
-  </si>
-  <si>
     <t>Fargo</t>
   </si>
   <si>
@@ -405,15 +399,6 @@
     <t>NoAuth</t>
   </si>
   <si>
-    <t>AddProgramId</t>
-  </si>
-  <si>
-    <t>AddProgramId,InvalidUri</t>
-  </si>
-  <si>
-    <t>AddProgramId,NoAuth</t>
-  </si>
-  <si>
     <t>Test Case</t>
   </si>
   <si>
@@ -493,6 +478,21 @@
   </si>
   <si>
     <t>Invalid - No Auth</t>
+  </si>
+  <si>
+    <t>/allProgramsWithUsersInvalid</t>
+  </si>
+  <si>
+    <t>validateSchemaProgram</t>
+  </si>
+  <si>
+    <t>InvalidUri</t>
+  </si>
+  <si>
+    <t>WellsTCNINE</t>
+  </si>
+  <si>
+    <t>testerTCNINE</t>
   </si>
 </sst>
 </file>
@@ -975,51 +975,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" t="s">
         <v>128</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" t="s">
         <v>129</v>
-      </c>
-      <c r="C1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D2">
         <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H2" t="s">
         <v>36</v>
@@ -1027,65 +1027,65 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D3">
         <v>401</v>
       </c>
       <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" t="s">
         <v>138</v>
       </c>
-      <c r="F3" t="s">
-        <v>143</v>
-      </c>
       <c r="H3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D4">
         <v>400</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D5">
         <v>200</v>
       </c>
       <c r="G5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -1093,39 +1093,39 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D6">
         <v>404</v>
       </c>
       <c r="G6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D7">
         <v>401</v>
       </c>
       <c r="H7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1382,7 +1382,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>1</v>
@@ -1431,13 +1431,13 @@
         <v>83</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>46</v>
@@ -1459,7 +1459,7 @@
         <v>84</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>33</v>
@@ -1689,7 +1689,9 @@
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6" t="s">
         <v>36</v>
@@ -1729,7 +1731,7 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>65</v>
@@ -1749,7 +1751,7 @@
         <v>73</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="8" t="s">
@@ -1769,8 +1771,8 @@
       <c r="F16" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>125</v>
+      <c r="G16" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="8" t="s">
@@ -1810,7 +1812,7 @@
         <v>77</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6" t="s">
@@ -1831,7 +1833,7 @@
         <v>77</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="8" t="s">
@@ -1870,7 +1872,9 @@
       <c r="F21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="8"/>
+      <c r="G21" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="H21" s="6"/>
       <c r="I21" s="8" t="s">
         <v>36</v>
@@ -1887,7 +1891,7 @@
         <v>58</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="6"/>
@@ -1910,7 +1914,7 @@
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>65</v>
@@ -1930,7 +1934,7 @@
         <v>82</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="8" t="s">
@@ -1942,13 +1946,13 @@
         <v>107</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Adding changes while merging
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A72B2DC-C4E9-4636-844C-4F5350AA7388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CC4CCC-2531-4F28-B3AF-4E9B35EE83EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="183">
   <si>
     <t>TestCase</t>
   </si>
@@ -383,23 +383,206 @@
     <t>tester</t>
   </si>
   <si>
-    <t>RubyAPI</t>
-  </si>
-  <si>
-    <t>TestS</t>
-  </si>
-  <si>
-    <t>Wells</t>
-  </si>
-  <si>
-    <t>Fargo</t>
+    <t>PUT_PROGRAM_08</t>
+  </si>
+  <si>
+    <t>Classs</t>
+  </si>
+  <si>
+    <t>Update Program by Name with Additional details</t>
+  </si>
+  <si>
+    <t>Update Program by Name with Mandatory details</t>
+  </si>
+  <si>
+    <t>program/abc@#</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>TestY</t>
+  </si>
+  <si>
+    <t>Update with missing mandatory fields in request body</t>
+  </si>
+  <si>
+    <t>Invalid values in request body</t>
+  </si>
+  <si>
+    <t>3435</t>
+  </si>
+  <si>
+    <t>%^^&amp;</t>
+  </si>
+  <si>
+    <t>TestQ123</t>
+  </si>
+  <si>
+    <t>TestQ@#$9999</t>
+  </si>
+  <si>
+    <t>Invalid Program Description</t>
+  </si>
+  <si>
+    <t>Valid - Update program status</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Invalid - No Auth</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_01</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_02</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_03</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_04</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_05</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_06</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_07</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_08</t>
+  </si>
+  <si>
+    <t>putprogram/{programId}</t>
+  </si>
+  <si>
+    <t>ClassDesc</t>
+  </si>
+  <si>
+    <t>Update Program by ID with Additional details</t>
+  </si>
+  <si>
+    <t>Update Program by ID with Mandatory details</t>
+  </si>
+  <si>
+    <t>putprogram/999999999999999999</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_09</t>
+  </si>
+  <si>
+    <t>Invalid Method to update program - Mentioned in Feature file</t>
+  </si>
+  <si>
+    <t>PUT_PROGRAM_ID_10</t>
+  </si>
+  <si>
+    <t>DEL_PROGRAM_ID_01</t>
+  </si>
+  <si>
+    <t>DEL_PROGRAM_ID_02</t>
+  </si>
+  <si>
+    <t>DEL_PROGRAM_ID_03</t>
+  </si>
+  <si>
+    <t>DEL_PROGRAM_NAME_01</t>
+  </si>
+  <si>
+    <t>DEL_PROGRAM_NAME_02</t>
+  </si>
+  <si>
+    <t>DEL_PROGRAM_NAME_03</t>
+  </si>
+  <si>
+    <t>/deletebyprogid/{programId}</t>
+  </si>
+  <si>
+    <t>/deletebyprogname/{programName}</t>
+  </si>
+  <si>
+    <t>Valid Delete Program by ID with Additional details</t>
+  </si>
+  <si>
+    <t>/deletebyprogid/@#$%^</t>
+  </si>
+  <si>
+    <t>Invalid -Delete with invalid Program by ID</t>
+  </si>
+  <si>
+    <t>Valid -Delete Program by Name with Additional details</t>
+  </si>
+  <si>
+    <t>Invalid -Delete with invalid Program by Name</t>
+  </si>
+  <si>
+    <t>desco</t>
+  </si>
+  <si>
+    <t>Invalid Update with missing mandatory fields in request body</t>
+  </si>
+  <si>
+    <t>Javaqw</t>
+  </si>
+  <si>
+    <t>APIAc</t>
+  </si>
+  <si>
+    <t>Javaac</t>
+  </si>
+  <si>
+    <t>Rubykc</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>NoAuth</t>
+  </si>
+  <si>
+    <t>AddProgramId</t>
+  </si>
+  <si>
+    <t>AddProgramId,InvalidUri</t>
+  </si>
+  <si>
+    <t>AddProgramId,NoAuth</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Rubyklb</t>
+  </si>
+  <si>
+    <t>Rubykor</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>csharpgh</t>
+  </si>
+  <si>
+    <t>Jetkdf</t>
+  </si>
+  <si>
+    <t>/deletebyprogname/0986hjhgyuf</t>
+  </si>
+  <si>
+    <t>csharpik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,8 +623,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,8 +649,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -532,12 +745,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -561,6 +807,54 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1083,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,11 +1390,12 @@
     <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="32.44140625" customWidth="1"/>
+    <col min="9" max="9" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -1120,15 +1415,21 @@
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>83</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>120</v>
+        <v>182</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>33</v>
@@ -1142,19 +1443,21 @@
       <c r="F2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="J2" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>121</v>
+        <v>180</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>33</v>
@@ -1166,14 +1469,16 @@
       <c r="F3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>85</v>
       </c>
@@ -1192,11 +1497,13 @@
       <c r="F4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>86</v>
       </c>
@@ -1215,11 +1522,13 @@
       <c r="F5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>87</v>
       </c>
@@ -1238,11 +1547,13 @@
       <c r="F6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>88</v>
       </c>
@@ -1261,11 +1572,13 @@
       <c r="F7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>89</v>
       </c>
@@ -1284,11 +1597,13 @@
       <c r="F8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>90</v>
       </c>
@@ -1303,11 +1618,13 @@
       <c r="F9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>91</v>
       </c>
@@ -1326,11 +1643,13 @@
       <c r="F10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>92</v>
       </c>
@@ -1349,11 +1668,13 @@
       <c r="F11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>93</v>
       </c>
@@ -1366,11 +1687,13 @@
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>94</v>
       </c>
@@ -1383,11 +1706,13 @@
       <c r="F13" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>95</v>
       </c>
@@ -1400,11 +1725,15 @@
       <c r="F14" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>96</v>
       </c>
@@ -1417,11 +1746,15 @@
       <c r="F15" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>97</v>
       </c>
@@ -1434,11 +1767,15 @@
       <c r="F16" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>98</v>
       </c>
@@ -1451,11 +1788,13 @@
       <c r="F17" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="43"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>99</v>
       </c>
@@ -1468,11 +1807,15 @@
       <c r="F18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>100</v>
       </c>
@@ -1485,11 +1828,15 @@
       <c r="F19" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>101</v>
       </c>
@@ -1502,11 +1849,13 @@
       <c r="F20" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="43"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>102</v>
       </c>
@@ -1519,11 +1868,13 @@
       <c r="F21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="43"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>103</v>
       </c>
@@ -1536,11 +1887,13 @@
       <c r="F22" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="43"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>104</v>
       </c>
@@ -1553,11 +1906,15 @@
       <c r="F23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="43"/>
+      <c r="H23" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>105</v>
       </c>
@@ -1570,16 +1927,20 @@
       <c r="F24" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>33</v>
@@ -1593,128 +1954,556 @@
       <c r="F25" s="11" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="11">
-        <v>1234</v>
+      <c r="D26" s="11" t="s">
+        <v>164</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>54</v>
+      <c r="B27" s="12" t="s">
+        <v>179</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11" t="s">
-        <v>46</v>
+        <v>133</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>57</v>
+        <v>124</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>63</v>
+      <c r="B29" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F29" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>112</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>113</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E32" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="36"/>
+      <c r="E34" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="H36" s="34"/>
+      <c r="I36" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H41" s="34"/>
+      <c r="I41" s="36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>52</v>
+      <c r="F42" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" s="20"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="26"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="G45" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="H45" s="39"/>
+      <c r="I45" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="26"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="H48" s="22"/>
+      <c r="I48" s="24" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{1ABA59E8-9459-41C9-BF54-78391EB45490}"/>
+    <hyperlink ref="F29" r:id="rId2" xr:uid="{4D2510A8-FACB-4347-A9E8-B307B8604CFB}"/>
+    <hyperlink ref="D31" r:id="rId3" xr:uid="{E68B04D2-6C43-4197-9821-1FDBD46D7752}"/>
+    <hyperlink ref="D40" r:id="rId4" xr:uid="{CCD63FD5-FC4B-49B0-8E85-6D9DBA0A7F3B}"/>
+    <hyperlink ref="F44" r:id="rId5" xr:uid="{E4310F2F-9C92-4A04-BCA3-0851479780EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding test data file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE214BA-873B-4356-BE59-12B411B1858D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540C8AA4-8F95-4E99-B9FF-92D4F574725F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1378,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added 2 more test cases to create program
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6426115-4431-4E95-88E7-A8ECC2EBAECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BF3507-5114-4EA4-83DB-1259397C52BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn-LogOut" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="213">
   <si>
     <t>TestCase</t>
   </si>
@@ -579,9 +579,6 @@
     <t>csharpsdf</t>
   </si>
   <si>
-    <t>Jetpoi</t>
-  </si>
-  <si>
     <t>Test Case</t>
   </si>
   <si>
@@ -658,6 +655,18 @@
   </si>
   <si>
     <t>GET_LOGOUT-06</t>
+  </si>
+  <si>
+    <t>analyticsdataa</t>
+  </si>
+  <si>
+    <t>bindera</t>
+  </si>
+  <si>
+    <t>POST_PROGRAM_11</t>
+  </si>
+  <si>
+    <t>POST_PROGRAM_12</t>
   </si>
 </sst>
 </file>
@@ -871,7 +880,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -939,7 +948,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1229,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16A0C37-AC78-46A6-A899-630BE249D064}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1246,166 +1254,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="C1" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" t="s">
         <v>186</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="F1" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="G1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" t="s">
         <v>189</v>
       </c>
-      <c r="G1" s="43" t="s">
-        <v>170</v>
-      </c>
-      <c r="H1" s="43" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="B2" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="43">
+      <c r="F2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3">
+        <v>401</v>
+      </c>
+      <c r="E3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>200</v>
       </c>
-      <c r="E2" s="43" t="s">
-        <v>194</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>195</v>
-      </c>
-      <c r="G2" s="43" t="s">
-        <v>196</v>
-      </c>
-      <c r="H2" s="43" t="s">
+      <c r="B4" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="E4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" t="s">
+        <v>201</v>
+      </c>
+      <c r="H4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="G5" t="s">
+        <v>205</v>
+      </c>
+      <c r="H5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="43">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6">
+        <v>404</v>
+      </c>
+      <c r="G6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7">
         <v>401</v>
       </c>
-      <c r="E3" s="43" t="s">
-        <v>194</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
-        <v>201</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" s="43">
-        <v>400</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>194</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>202</v>
-      </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="43">
-        <v>200</v>
-      </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
-        <v>207</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>208</v>
-      </c>
-      <c r="D6" s="43">
-        <v>404</v>
-      </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
-        <v>209</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="D7" s="43">
-        <v>401</v>
-      </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43" t="s">
+      <c r="H7" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1660,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1712,7 +1711,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>33</v>
@@ -1740,7 +1739,7 @@
         <v>84</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>33</v>
@@ -1762,78 +1761,84 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="11">
-        <v>1234</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>50</v>
+      <c r="D4" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
-        <v>61</v>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>57</v>
+      <c r="D5" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11" t="s">
-        <v>71</v>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>63</v>
+      <c r="B6" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>58</v>
+      <c r="D6" s="11">
+        <v>1234</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1841,7 +1846,7 @@
         <v>88</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>33</v>
@@ -1849,8 +1854,8 @@
       <c r="D7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>50</v>
+      <c r="E7" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>52</v>
@@ -1858,7 +1863,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1866,7 +1871,7 @@
         <v>89</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>33</v>
@@ -1874,28 +1879,32 @@
       <c r="D8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>75</v>
+      <c r="E8" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="B9" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="11" t="s">
@@ -1904,15 +1913,15 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>67</v>
+      <c r="B10" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>33</v>
@@ -1921,7 +1930,7 @@
         <v>56</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>52</v>
@@ -1929,21 +1938,17 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>56</v>
+      <c r="B11" s="12"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>50</v>
@@ -1954,176 +1959,184 @@
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
-        <v>173</v>
-      </c>
+      <c r="G14" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="6"/>
       <c r="I14" s="6" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>171</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="8" t="s">
-        <v>76</v>
+      <c r="I15" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8" t="s">
-        <v>36</v>
+        <v>75</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="6" t="s">
-        <v>79</v>
+        <v>57</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="7" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="6" t="s">
-        <v>80</v>
+      <c r="I18" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>171</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="G19" s="8"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="8" t="s">
-        <v>76</v>
+      <c r="I19" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -2132,38 +2145,40 @@
         <v>58</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="H20" s="8"/>
-      <c r="I20" s="8" t="s">
-        <v>60</v>
+      <c r="I20" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="7" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2172,7 +2187,7 @@
         <v>58</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>181</v>
+        <v>81</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -2182,110 +2197,100 @@
     </row>
     <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="6" t="s">
-        <v>173</v>
-      </c>
+      <c r="G23" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H23" s="8"/>
       <c r="I23" s="8" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>171</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F27" s="11" t="s">
@@ -2293,70 +2298,70 @@
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="29" t="s">
-        <v>132</v>
+      <c r="I27" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+        <v>108</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="D28" s="11" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>114</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
-      <c r="I28" s="11" t="s">
-        <v>165</v>
+      <c r="I28" s="8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>54</v>
+        <v>109</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
+        <v>133</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
       <c r="I29" s="29" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>128</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="11" t="s">
@@ -2364,50 +2369,50 @@
       </c>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
-      <c r="I30" s="29" t="s">
-        <v>126</v>
+      <c r="I30" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>63</v>
+        <v>111</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="D31" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
       <c r="I31" s="29" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>57</v>
+        <v>129</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>114</v>
@@ -2415,71 +2420,73 @@
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="I32" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="29" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="31" t="s">
+    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B35" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C35" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D35" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="E33" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="35" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="35" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="B35" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="E35" s="38" t="s">
+      <c r="E35" s="33" t="s">
         <v>72</v>
       </c>
       <c r="F35" s="34" t="s">
@@ -2487,120 +2494,118 @@
       </c>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
-      <c r="I35" s="36" t="s">
-        <v>132</v>
+      <c r="I35" s="35" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>174</v>
+        <v>136</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>168</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="38" t="s">
-        <v>58</v>
+      <c r="D36" s="36"/>
+      <c r="E36" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="F36" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="G36" s="35" t="s">
-        <v>172</v>
-      </c>
+      <c r="G36" s="34"/>
       <c r="H36" s="34"/>
-      <c r="I36" s="36" t="s">
-        <v>80</v>
+      <c r="I36" s="35" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="B37" s="36" t="s">
-        <v>54</v>
+        <v>137</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>169</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="E37" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="17" t="s">
-        <v>79</v>
+        <v>133</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="36" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="37" t="s">
-        <v>50</v>
+        <v>138</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="F38" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="17" t="s">
-        <v>125</v>
+      <c r="G38" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="H38" s="34"/>
+      <c r="I38" s="36" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="B39" s="40" t="s">
-        <v>127</v>
+        <v>139</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>54</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>128</v>
+        <v>33</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>143</v>
+        <v>123</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
       <c r="I39" s="17" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="B40" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C40" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="E40" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="37" t="s">
         <v>50</v>
       </c>
       <c r="F40" s="34" t="s">
@@ -2609,188 +2614,238 @@
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
       <c r="I40" s="17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="36" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B41" s="40" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="37" t="s">
-        <v>57</v>
+        <v>129</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>50</v>
       </c>
       <c r="F41" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="G41" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="H41" s="34"/>
-      <c r="I41" s="36" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="42" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="36" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>63</v>
+        <v>175</v>
       </c>
       <c r="C42" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="36" t="s">
-        <v>56</v>
+      <c r="D42" s="41" t="s">
+        <v>130</v>
       </c>
       <c r="E42" s="38" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F42" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34" t="s">
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G43" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H43" s="34"/>
+      <c r="I43" s="36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="42" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="I42" s="36" t="s">
+      <c r="I44" s="36" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="19" t="s">
+    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="21" t="s">
+      <c r="B45" s="20"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="21" t="s">
         <v>72</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F44" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="B45" s="26"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="27" t="s">
-        <v>57</v>
       </c>
       <c r="F45" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="G45" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="H45" s="39"/>
-      <c r="I45" s="28" t="s">
-        <v>134</v>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="23" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
+      <c r="A46" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
       <c r="I46" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="B47" s="24"/>
+        <v>153</v>
+      </c>
+      <c r="B47" s="26"/>
       <c r="C47" s="24"/>
       <c r="D47" s="24"/>
-      <c r="E47" s="25" t="s">
-        <v>58</v>
+      <c r="E47" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="23" t="s">
-        <v>163</v>
+        <v>157</v>
+      </c>
+      <c r="G47" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47" s="39"/>
+      <c r="I47" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="27" t="s">
-        <v>57</v>
+      <c r="A48" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="21" t="s">
+        <v>72</v>
       </c>
       <c r="F48" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="G48" s="22" t="s">
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" s="26"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="G50" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="H48" s="22"/>
-      <c r="I48" s="24" t="s">
+      <c r="H50" s="22"/>
+      <c r="I50" s="24" t="s">
         <v>134</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{1ABA59E8-9459-41C9-BF54-78391EB45490}"/>
-    <hyperlink ref="F29" r:id="rId2" xr:uid="{4D2510A8-FACB-4347-A9E8-B307B8604CFB}"/>
-    <hyperlink ref="D31" r:id="rId3" xr:uid="{E68B04D2-6C43-4197-9821-1FDBD46D7752}"/>
-    <hyperlink ref="D40" r:id="rId4" xr:uid="{CCD63FD5-FC4B-49B0-8E85-6D9DBA0A7F3B}"/>
-    <hyperlink ref="F44" r:id="rId5" xr:uid="{E4310F2F-9C92-4A04-BCA3-0851479780EC}"/>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{1ABA59E8-9459-41C9-BF54-78391EB45490}"/>
+    <hyperlink ref="F31" r:id="rId2" xr:uid="{4D2510A8-FACB-4347-A9E8-B307B8604CFB}"/>
+    <hyperlink ref="D33" r:id="rId3" xr:uid="{E68B04D2-6C43-4197-9821-1FDBD46D7752}"/>
+    <hyperlink ref="D42" r:id="rId4" xr:uid="{CCD63FD5-FC4B-49B0-8E85-6D9DBA0A7F3B}"/>
+    <hyperlink ref="F46" r:id="rId5" xr:uid="{E4310F2F-9C92-4A04-BCA3-0851479780EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commiting Batch module changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anbum\OneDrive\Desktop\Anbu\LMS_Phase2_RestAssured\LMS_GIT\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anbum\OneDrive\Desktop\Anbu\LMS_Phase2_RestAssured\GitRECOVERY\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EA9D5E-B109-4ABE-958A-82BC74C328B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5009C81-2D79-449A-86A3-BC074334530B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1366,22 +1366,22 @@
     <t>All Valid data</t>
   </si>
   <si>
-    <t>binxeq</t>
-  </si>
-  <si>
-    <t>analytapgfgdfdyrrfddffd</t>
-  </si>
-  <si>
-    <t>analyticytgfdgdefdfdknd</t>
-  </si>
-  <si>
-    <t>analytdpgfgddhgrc fdfdmb</t>
-  </si>
-  <si>
-    <t>analytic49</t>
-  </si>
-  <si>
-    <t>analytic50</t>
+    <t>bestFOanalytica</t>
+  </si>
+  <si>
+    <t>bestanalica</t>
+  </si>
+  <si>
+    <t>bestTbinxq</t>
+  </si>
+  <si>
+    <t>bestTHanytica</t>
+  </si>
+  <si>
+    <t>anatic98</t>
+  </si>
+  <si>
+    <t>anatic97</t>
   </si>
 </sst>
 </file>
@@ -2175,7 +2175,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3167,7 +3167,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,7 +3244,7 @@
         <v>77</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>27</v>
@@ -3270,7 +3270,7 @@
         <v>78</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>27</v>
@@ -3298,7 +3298,7 @@
         <v>79</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Final commit to main (updated)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A25D4B-C75E-45C1-BA2E-9EEAC99D4B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0137C41-3C30-4E52-9038-9B7D0C9D6468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn-LogOut" sheetId="4" r:id="rId1"/>
@@ -1699,46 +1699,46 @@
     <t>validateSchemaProgramArray</t>
   </si>
   <si>
-    <t>apiavengersteamprogmmm</t>
-  </si>
-  <si>
-    <t>apiavengersteamproggmandatory</t>
-  </si>
-  <si>
-    <t>apiavengersteaamfourprogthree</t>
-  </si>
-  <si>
-    <t>apiavengersteeamfourprogfour</t>
-  </si>
-  <si>
-    <t>apiavengeersteamputname</t>
-  </si>
-  <si>
-    <t>apiavpuutname</t>
-  </si>
-  <si>
-    <t>apiaveengersteamfourputname</t>
-  </si>
-  <si>
-    <t>apiavvengersteamputidone</t>
-  </si>
-  <si>
-    <t>apiavpputidone</t>
-  </si>
-  <si>
-    <t>apiavenngersteamfourputidone</t>
-  </si>
-  <si>
-    <t>apiavgbatchteam004</t>
-  </si>
-  <si>
-    <t>batchapiavengerrsteam04h</t>
-  </si>
-  <si>
-    <t>apiavengerfourthteaamm</t>
-  </si>
-  <si>
-    <t>Pythonclassstopicapiavg1</t>
+    <t>apiavengersteamproggm</t>
+  </si>
+  <si>
+    <t>apiavengersteamproogmandatory</t>
+  </si>
+  <si>
+    <t>apiavengersteaamfourprogg</t>
+  </si>
+  <si>
+    <t>apiavengerstteamfourprogfour</t>
+  </si>
+  <si>
+    <t>apiavengerssteamputname</t>
+  </si>
+  <si>
+    <t>apiavputnname</t>
+  </si>
+  <si>
+    <t>apiiavengersteamfourputname</t>
+  </si>
+  <si>
+    <t>apiavvengersteamputidd</t>
+  </si>
+  <si>
+    <t>apiavpputidonee</t>
+  </si>
+  <si>
+    <t>apiavenggersteamfourputidone</t>
+  </si>
+  <si>
+    <t>apiavgbatchteam4</t>
+  </si>
+  <si>
+    <t>batchapiavengersteam4</t>
+  </si>
+  <si>
+    <t>apiavengerrfourthteam</t>
+  </si>
+  <si>
+    <t>Pythonclassttopicapiavg1</t>
   </si>
 </sst>
 </file>
@@ -2569,7 +2569,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3560,14 +3560,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71699B68-ACC9-4CEF-899B-01EDAE8A191D}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
@@ -4753,8 +4753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF50A04-6C24-4538-A7F6-001CEB342DEB}">
   <dimension ref="A1:AD1009"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
commiting updated test data to main
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\Team04_APIAvengers_LMSHackathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0137C41-3C30-4E52-9038-9B7D0C9D6468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC0A3F5-9CE0-4644-81A4-D0C9B2A09D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn-LogOut" sheetId="4" r:id="rId1"/>
@@ -1699,46 +1699,46 @@
     <t>validateSchemaProgramArray</t>
   </si>
   <si>
-    <t>apiavengersteamproggm</t>
-  </si>
-  <si>
-    <t>apiavengersteamproogmandatory</t>
-  </si>
-  <si>
-    <t>apiavengersteaamfourprogg</t>
-  </si>
-  <si>
-    <t>apiavengerstteamfourprogfour</t>
-  </si>
-  <si>
-    <t>apiavengerssteamputname</t>
-  </si>
-  <si>
-    <t>apiavputnname</t>
-  </si>
-  <si>
-    <t>apiiavengersteamfourputname</t>
-  </si>
-  <si>
-    <t>apiavvengersteamputidd</t>
-  </si>
-  <si>
-    <t>apiavpputidonee</t>
-  </si>
-  <si>
-    <t>apiavenggersteamfourputidone</t>
-  </si>
-  <si>
-    <t>apiavgbatchteam4</t>
-  </si>
-  <si>
-    <t>batchapiavengersteam4</t>
-  </si>
-  <si>
-    <t>apiavengerrfourthteam</t>
-  </si>
-  <si>
-    <t>Pythonclassttopicapiavg1</t>
+    <t>apiavengers04</t>
+  </si>
+  <si>
+    <t>batchavengers04</t>
+  </si>
+  <si>
+    <t>apiavengersss</t>
+  </si>
+  <si>
+    <t>apiavengeersteamproggg</t>
+  </si>
+  <si>
+    <t>aapiavengersfourrrprog</t>
+  </si>
+  <si>
+    <t>apiavengerrrfourprr</t>
+  </si>
+  <si>
+    <t>apiavengerteamputone</t>
+  </si>
+  <si>
+    <t>apiavputnametwo</t>
+  </si>
+  <si>
+    <t>apiaavengersteamfourputthree</t>
+  </si>
+  <si>
+    <t>apiaavenngersteamputidone</t>
+  </si>
+  <si>
+    <t>apiavpputidtwoo</t>
+  </si>
+  <si>
+    <t>apiavenggersteamfourputidthreee</t>
+  </si>
+  <si>
+    <t>apiavengerrtfourone</t>
+  </si>
+  <si>
+    <t>Pythonclastopicapitwo</t>
   </si>
 </sst>
 </file>
@@ -2830,7 +2830,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>25</v>
@@ -2930,7 +2930,7 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D13" t="s">
         <v>398</v>
@@ -3610,7 +3610,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>26</v>
@@ -3638,7 +3638,7 @@
         <v>76</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>26</v>
@@ -3664,7 +3664,7 @@
         <v>77</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>26</v>
@@ -3692,7 +3692,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>26</v>
@@ -4181,7 +4181,7 @@
         <v>99</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>26</v>
@@ -4206,7 +4206,7 @@
         <v>100</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>26</v>
@@ -4231,7 +4231,7 @@
         <v>101</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>26</v>
@@ -4377,7 +4377,7 @@
         <v>127</v>
       </c>
       <c r="B35" s="56" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C35" s="31" t="s">
         <v>26</v>
@@ -4402,7 +4402,7 @@
         <v>128</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>26</v>
@@ -4425,7 +4425,7 @@
         <v>129</v>
       </c>
       <c r="B37" s="56" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C37" s="36" t="s">
         <v>125</v>
@@ -4754,7 +4754,7 @@
   <dimension ref="A1:AD1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>